<commit_message>
Update on 20250415 part 6
</commit_message>
<xml_diff>
--- a/直播源汇总文档/高码和BPTV/肥羊高码和BPTV.xlsx
+++ b/直播源汇总文档/高码和BPTV/肥羊高码和BPTV.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">bptv!$A$1:$E$205</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">bptv!$A$1:$E$217</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">高码!$A$1:$E$157</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2272" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2272" uniqueCount="160">
   <si>
     <t>湖南卫视</t>
   </si>
@@ -510,6 +510,10 @@
   </si>
   <si>
     <t>/bptv/10000100000000050000000003887500.m3u8</t>
+  </si>
+  <si>
+    <t>北京卫视</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -3795,7 +3799,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>64</v>
+        <v>159</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>69</v>
@@ -3803,16 +3807,16 @@
       <c r="C14" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>71</v>
+      <c r="D14" t="s">
+        <v>139</v>
       </c>
       <c r="E14" t="s">
-        <v>65</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>159</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>69</v>
@@ -3820,16 +3824,16 @@
       <c r="C15" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>82</v>
+      <c r="D15" t="s">
+        <v>81</v>
       </c>
       <c r="E15" t="s">
-        <v>65</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>64</v>
+        <v>159</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>69</v>
@@ -3837,16 +3841,16 @@
       <c r="C16" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>86</v>
+      <c r="D16" t="s">
+        <v>83</v>
       </c>
       <c r="E16" t="s">
-        <v>65</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>64</v>
+        <v>159</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>69</v>
@@ -3854,16 +3858,16 @@
       <c r="C17" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>85</v>
+      <c r="D17" t="s">
+        <v>84</v>
       </c>
       <c r="E17" t="s">
-        <v>65</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>64</v>
+        <v>159</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>69</v>
@@ -3871,16 +3875,16 @@
       <c r="C18" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>80</v>
+      <c r="D18" t="s">
+        <v>79</v>
       </c>
       <c r="E18" t="s">
-        <v>65</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>64</v>
+        <v>159</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>69</v>
@@ -3888,16 +3892,16 @@
       <c r="C19" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>78</v>
+      <c r="D19" t="s">
+        <v>77</v>
       </c>
       <c r="E19" t="s">
-        <v>65</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>69</v>
@@ -3905,16 +3909,16 @@
       <c r="C20" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>71</v>
+      <c r="D20" t="s">
+        <v>139</v>
       </c>
       <c r="E20" t="s">
-        <v>33</v>
+        <v>151</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>69</v>
@@ -3922,16 +3926,16 @@
       <c r="C21" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>82</v>
+      <c r="D21" t="s">
+        <v>81</v>
       </c>
       <c r="E21" t="s">
-        <v>33</v>
+        <v>151</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>69</v>
@@ -3939,16 +3943,16 @@
       <c r="C22" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>86</v>
+      <c r="D22" t="s">
+        <v>83</v>
       </c>
       <c r="E22" t="s">
-        <v>33</v>
+        <v>151</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>69</v>
@@ -3956,16 +3960,16 @@
       <c r="C23" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>85</v>
+      <c r="D23" t="s">
+        <v>84</v>
       </c>
       <c r="E23" t="s">
-        <v>33</v>
+        <v>151</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>69</v>
@@ -3973,16 +3977,16 @@
       <c r="C24" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>80</v>
+      <c r="D24" t="s">
+        <v>79</v>
       </c>
       <c r="E24" t="s">
-        <v>33</v>
+        <v>151</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>69</v>
@@ -3990,16 +3994,16 @@
       <c r="C25" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>78</v>
+      <c r="D25" t="s">
+        <v>77</v>
       </c>
       <c r="E25" t="s">
-        <v>33</v>
+        <v>151</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>69</v>
@@ -4011,12 +4015,12 @@
         <v>71</v>
       </c>
       <c r="E26" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>69</v>
@@ -4028,12 +4032,12 @@
         <v>82</v>
       </c>
       <c r="E27" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>69</v>
@@ -4045,12 +4049,12 @@
         <v>86</v>
       </c>
       <c r="E28" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>69</v>
@@ -4062,12 +4066,12 @@
         <v>85</v>
       </c>
       <c r="E29" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>69</v>
@@ -4079,12 +4083,12 @@
         <v>80</v>
       </c>
       <c r="E30" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>69</v>
@@ -4096,12 +4100,12 @@
         <v>78</v>
       </c>
       <c r="E31" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>69</v>
@@ -4113,12 +4117,12 @@
         <v>71</v>
       </c>
       <c r="E32" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>69</v>
@@ -4130,12 +4134,12 @@
         <v>82</v>
       </c>
       <c r="E33" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>69</v>
@@ -4147,12 +4151,12 @@
         <v>86</v>
       </c>
       <c r="E34" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>69</v>
@@ -4164,12 +4168,12 @@
         <v>85</v>
       </c>
       <c r="E35" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>69</v>
@@ -4181,12 +4185,12 @@
         <v>80</v>
       </c>
       <c r="E36" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>69</v>
@@ -4198,12 +4202,12 @@
         <v>78</v>
       </c>
       <c r="E37" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>69</v>
@@ -4215,12 +4219,12 @@
         <v>71</v>
       </c>
       <c r="E38" t="s">
-        <v>53</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>69</v>
@@ -4232,12 +4236,12 @@
         <v>82</v>
       </c>
       <c r="E39" t="s">
-        <v>53</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>69</v>
@@ -4249,12 +4253,12 @@
         <v>86</v>
       </c>
       <c r="E40" t="s">
-        <v>53</v>
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>69</v>
@@ -4266,12 +4270,12 @@
         <v>85</v>
       </c>
       <c r="E41" t="s">
-        <v>53</v>
+        <v>7</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>69</v>
@@ -4283,12 +4287,12 @@
         <v>80</v>
       </c>
       <c r="E42" t="s">
-        <v>53</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>69</v>
@@ -4300,12 +4304,12 @@
         <v>78</v>
       </c>
       <c r="E43" t="s">
-        <v>53</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>69</v>
@@ -4317,12 +4321,12 @@
         <v>71</v>
       </c>
       <c r="E44" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>69</v>
@@ -4334,12 +4338,12 @@
         <v>82</v>
       </c>
       <c r="E45" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>69</v>
@@ -4351,12 +4355,12 @@
         <v>86</v>
       </c>
       <c r="E46" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>69</v>
@@ -4368,12 +4372,12 @@
         <v>85</v>
       </c>
       <c r="E47" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>69</v>
@@ -4385,12 +4389,12 @@
         <v>80</v>
       </c>
       <c r="E48" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>69</v>
@@ -4402,12 +4406,12 @@
         <v>78</v>
       </c>
       <c r="E49" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>69</v>
@@ -4419,12 +4423,12 @@
         <v>71</v>
       </c>
       <c r="E50" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>69</v>
@@ -4436,12 +4440,12 @@
         <v>82</v>
       </c>
       <c r="E51" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A52" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>69</v>
@@ -4453,12 +4457,12 @@
         <v>86</v>
       </c>
       <c r="E52" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A53" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>69</v>
@@ -4470,12 +4474,12 @@
         <v>85</v>
       </c>
       <c r="E53" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A54" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>69</v>
@@ -4487,12 +4491,12 @@
         <v>80</v>
       </c>
       <c r="E54" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A55" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>69</v>
@@ -4504,12 +4508,12 @@
         <v>78</v>
       </c>
       <c r="E55" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A56" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>69</v>
@@ -4521,12 +4525,12 @@
         <v>71</v>
       </c>
       <c r="E56" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A57" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>69</v>
@@ -4538,12 +4542,12 @@
         <v>82</v>
       </c>
       <c r="E57" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A58" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>69</v>
@@ -4555,12 +4559,12 @@
         <v>86</v>
       </c>
       <c r="E58" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A59" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>69</v>
@@ -4572,12 +4576,12 @@
         <v>85</v>
       </c>
       <c r="E59" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A60" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>69</v>
@@ -4589,12 +4593,12 @@
         <v>80</v>
       </c>
       <c r="E60" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A61" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>69</v>
@@ -4606,12 +4610,12 @@
         <v>78</v>
       </c>
       <c r="E61" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A62" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>69</v>
@@ -4623,12 +4627,12 @@
         <v>71</v>
       </c>
       <c r="E62" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A63" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>69</v>
@@ -4640,12 +4644,12 @@
         <v>82</v>
       </c>
       <c r="E63" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A64" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>69</v>
@@ -4657,12 +4661,12 @@
         <v>86</v>
       </c>
       <c r="E64" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A65" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>69</v>
@@ -4674,12 +4678,12 @@
         <v>85</v>
       </c>
       <c r="E65" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A66" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>69</v>
@@ -4691,12 +4695,12 @@
         <v>80</v>
       </c>
       <c r="E66" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A67" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>69</v>
@@ -4708,12 +4712,12 @@
         <v>78</v>
       </c>
       <c r="E67" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A68" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>69</v>
@@ -4725,12 +4729,12 @@
         <v>71</v>
       </c>
       <c r="E68" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A69" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>69</v>
@@ -4742,12 +4746,12 @@
         <v>82</v>
       </c>
       <c r="E69" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A70" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>69</v>
@@ -4759,12 +4763,12 @@
         <v>86</v>
       </c>
       <c r="E70" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A71" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>69</v>
@@ -4776,12 +4780,12 @@
         <v>85</v>
       </c>
       <c r="E71" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A72" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>69</v>
@@ -4793,12 +4797,12 @@
         <v>80</v>
       </c>
       <c r="E72" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A73" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>69</v>
@@ -4810,12 +4814,12 @@
         <v>78</v>
       </c>
       <c r="E73" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A74" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>69</v>
@@ -4827,12 +4831,12 @@
         <v>71</v>
       </c>
       <c r="E74" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A75" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>69</v>
@@ -4844,12 +4848,12 @@
         <v>82</v>
       </c>
       <c r="E75" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A76" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>69</v>
@@ -4861,12 +4865,12 @@
         <v>86</v>
       </c>
       <c r="E76" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A77" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>69</v>
@@ -4878,12 +4882,12 @@
         <v>85</v>
       </c>
       <c r="E77" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A78" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>69</v>
@@ -4895,12 +4899,12 @@
         <v>80</v>
       </c>
       <c r="E78" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A79" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>69</v>
@@ -4912,12 +4916,12 @@
         <v>78</v>
       </c>
       <c r="E79" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A80" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>69</v>
@@ -4929,12 +4933,12 @@
         <v>71</v>
       </c>
       <c r="E80" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A81" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>69</v>
@@ -4946,12 +4950,12 @@
         <v>82</v>
       </c>
       <c r="E81" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A82" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>69</v>
@@ -4963,12 +4967,12 @@
         <v>86</v>
       </c>
       <c r="E82" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A83" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>69</v>
@@ -4980,12 +4984,12 @@
         <v>85</v>
       </c>
       <c r="E83" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A84" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>69</v>
@@ -4997,12 +5001,12 @@
         <v>80</v>
       </c>
       <c r="E84" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A85" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>69</v>
@@ -5014,12 +5018,12 @@
         <v>78</v>
       </c>
       <c r="E85" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A86" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>69</v>
@@ -5031,12 +5035,12 @@
         <v>71</v>
       </c>
       <c r="E86" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A87" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>69</v>
@@ -5048,12 +5052,12 @@
         <v>82</v>
       </c>
       <c r="E87" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A88" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>69</v>
@@ -5065,12 +5069,12 @@
         <v>86</v>
       </c>
       <c r="E88" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A89" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>69</v>
@@ -5082,12 +5086,12 @@
         <v>85</v>
       </c>
       <c r="E89" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A90" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>69</v>
@@ -5099,12 +5103,12 @@
         <v>80</v>
       </c>
       <c r="E90" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A91" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>69</v>
@@ -5116,12 +5120,12 @@
         <v>78</v>
       </c>
       <c r="E91" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A92" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>69</v>
@@ -5133,12 +5137,12 @@
         <v>71</v>
       </c>
       <c r="E92" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A93" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>69</v>
@@ -5150,12 +5154,12 @@
         <v>82</v>
       </c>
       <c r="E93" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A94" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>69</v>
@@ -5167,12 +5171,12 @@
         <v>86</v>
       </c>
       <c r="E94" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A95" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>69</v>
@@ -5184,12 +5188,12 @@
         <v>85</v>
       </c>
       <c r="E95" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A96" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>69</v>
@@ -5201,12 +5205,12 @@
         <v>80</v>
       </c>
       <c r="E96" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A97" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>69</v>
@@ -5218,12 +5222,12 @@
         <v>78</v>
       </c>
       <c r="E97" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A98" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>69</v>
@@ -5235,12 +5239,12 @@
         <v>71</v>
       </c>
       <c r="E98" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A99" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>69</v>
@@ -5252,12 +5256,12 @@
         <v>82</v>
       </c>
       <c r="E99" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A100" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>69</v>
@@ -5269,12 +5273,12 @@
         <v>86</v>
       </c>
       <c r="E100" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A101" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>69</v>
@@ -5286,12 +5290,12 @@
         <v>85</v>
       </c>
       <c r="E101" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A102" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>69</v>
@@ -5303,12 +5307,12 @@
         <v>80</v>
       </c>
       <c r="E102" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A103" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>69</v>
@@ -5320,12 +5324,12 @@
         <v>78</v>
       </c>
       <c r="E103" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A104" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>69</v>
@@ -5337,12 +5341,12 @@
         <v>71</v>
       </c>
       <c r="E104" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A105" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>69</v>
@@ -5354,12 +5358,12 @@
         <v>82</v>
       </c>
       <c r="E105" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A106" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>69</v>
@@ -5371,12 +5375,12 @@
         <v>86</v>
       </c>
       <c r="E106" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A107" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>69</v>
@@ -5388,12 +5392,12 @@
         <v>85</v>
       </c>
       <c r="E107" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A108" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>69</v>
@@ -5405,12 +5409,12 @@
         <v>80</v>
       </c>
       <c r="E108" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A109" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>69</v>
@@ -5422,12 +5426,12 @@
         <v>78</v>
       </c>
       <c r="E109" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A110" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>69</v>
@@ -5439,12 +5443,12 @@
         <v>71</v>
       </c>
       <c r="E110" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A111" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>69</v>
@@ -5456,12 +5460,12 @@
         <v>82</v>
       </c>
       <c r="E111" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A112" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>69</v>
@@ -5473,12 +5477,12 @@
         <v>86</v>
       </c>
       <c r="E112" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A113" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>69</v>
@@ -5490,12 +5494,12 @@
         <v>85</v>
       </c>
       <c r="E113" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A114" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>69</v>
@@ -5507,12 +5511,12 @@
         <v>80</v>
       </c>
       <c r="E114" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A115" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>69</v>
@@ -5524,12 +5528,12 @@
         <v>78</v>
       </c>
       <c r="E115" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A116" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>69</v>
@@ -5541,12 +5545,12 @@
         <v>71</v>
       </c>
       <c r="E116" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A117" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>69</v>
@@ -5558,12 +5562,12 @@
         <v>82</v>
       </c>
       <c r="E117" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A118" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>69</v>
@@ -5575,12 +5579,12 @@
         <v>86</v>
       </c>
       <c r="E118" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A119" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>69</v>
@@ -5592,12 +5596,12 @@
         <v>85</v>
       </c>
       <c r="E119" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A120" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>69</v>
@@ -5609,12 +5613,12 @@
         <v>80</v>
       </c>
       <c r="E120" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A121" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>69</v>
@@ -5626,12 +5630,12 @@
         <v>78</v>
       </c>
       <c r="E121" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A122" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>69</v>
@@ -5643,12 +5647,12 @@
         <v>71</v>
       </c>
       <c r="E122" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A123" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>69</v>
@@ -5660,12 +5664,12 @@
         <v>82</v>
       </c>
       <c r="E123" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A124" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>69</v>
@@ -5677,12 +5681,12 @@
         <v>86</v>
       </c>
       <c r="E124" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A125" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>69</v>
@@ -5694,12 +5698,12 @@
         <v>85</v>
       </c>
       <c r="E125" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A126" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>69</v>
@@ -5711,12 +5715,12 @@
         <v>80</v>
       </c>
       <c r="E126" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A127" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>69</v>
@@ -5728,12 +5732,12 @@
         <v>78</v>
       </c>
       <c r="E127" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A128" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>69</v>
@@ -5745,12 +5749,12 @@
         <v>71</v>
       </c>
       <c r="E128" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A129" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>69</v>
@@ -5762,12 +5766,12 @@
         <v>82</v>
       </c>
       <c r="E129" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A130" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>69</v>
@@ -5779,12 +5783,12 @@
         <v>86</v>
       </c>
       <c r="E130" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A131" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>69</v>
@@ -5796,12 +5800,12 @@
         <v>85</v>
       </c>
       <c r="E131" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A132" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>69</v>
@@ -5813,12 +5817,12 @@
         <v>80</v>
       </c>
       <c r="E132" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A133" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>69</v>
@@ -5830,12 +5834,12 @@
         <v>78</v>
       </c>
       <c r="E133" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A134" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>69</v>
@@ -5847,12 +5851,12 @@
         <v>71</v>
       </c>
       <c r="E134" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A135" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>69</v>
@@ -5864,12 +5868,12 @@
         <v>82</v>
       </c>
       <c r="E135" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A136" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>69</v>
@@ -5881,12 +5885,12 @@
         <v>86</v>
       </c>
       <c r="E136" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A137" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>69</v>
@@ -5898,12 +5902,12 @@
         <v>85</v>
       </c>
       <c r="E137" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A138" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>69</v>
@@ -5915,12 +5919,12 @@
         <v>80</v>
       </c>
       <c r="E138" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A139" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>69</v>
@@ -5932,12 +5936,12 @@
         <v>78</v>
       </c>
       <c r="E139" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A140" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>69</v>
@@ -5949,12 +5953,12 @@
         <v>71</v>
       </c>
       <c r="E140" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A141" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>69</v>
@@ -5966,12 +5970,12 @@
         <v>82</v>
       </c>
       <c r="E141" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A142" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>69</v>
@@ -5983,12 +5987,12 @@
         <v>86</v>
       </c>
       <c r="E142" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A143" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>69</v>
@@ -6000,12 +6004,12 @@
         <v>85</v>
       </c>
       <c r="E143" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A144" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>69</v>
@@ -6017,12 +6021,12 @@
         <v>80</v>
       </c>
       <c r="E144" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A145" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>69</v>
@@ -6034,12 +6038,12 @@
         <v>78</v>
       </c>
       <c r="E145" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A146" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="B146" s="1" t="s">
         <v>69</v>
@@ -6051,12 +6055,12 @@
         <v>71</v>
       </c>
       <c r="E146" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A147" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="B147" s="1" t="s">
         <v>69</v>
@@ -6068,12 +6072,12 @@
         <v>82</v>
       </c>
       <c r="E147" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A148" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>69</v>
@@ -6085,12 +6089,12 @@
         <v>86</v>
       </c>
       <c r="E148" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A149" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>69</v>
@@ -6102,12 +6106,12 @@
         <v>85</v>
       </c>
       <c r="E149" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A150" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="B150" s="1" t="s">
         <v>69</v>
@@ -6119,12 +6123,12 @@
         <v>80</v>
       </c>
       <c r="E150" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A151" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>69</v>
@@ -6136,12 +6140,12 @@
         <v>78</v>
       </c>
       <c r="E151" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A152" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>69</v>
@@ -6153,12 +6157,12 @@
         <v>71</v>
       </c>
       <c r="E152" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A153" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="B153" s="1" t="s">
         <v>69</v>
@@ -6170,12 +6174,12 @@
         <v>82</v>
       </c>
       <c r="E153" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A154" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="B154" s="1" t="s">
         <v>69</v>
@@ -6187,12 +6191,12 @@
         <v>86</v>
       </c>
       <c r="E154" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A155" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="B155" s="1" t="s">
         <v>69</v>
@@ -6204,12 +6208,12 @@
         <v>85</v>
       </c>
       <c r="E155" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A156" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="B156" s="1" t="s">
         <v>69</v>
@@ -6221,12 +6225,12 @@
         <v>80</v>
       </c>
       <c r="E156" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A157" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="B157" s="1" t="s">
         <v>69</v>
@@ -6238,12 +6242,12 @@
         <v>78</v>
       </c>
       <c r="E157" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A158" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>69</v>
@@ -6255,12 +6259,12 @@
         <v>71</v>
       </c>
       <c r="E158" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A159" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="B159" s="1" t="s">
         <v>69</v>
@@ -6272,12 +6276,12 @@
         <v>82</v>
       </c>
       <c r="E159" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A160" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="B160" s="1" t="s">
         <v>69</v>
@@ -6289,12 +6293,12 @@
         <v>86</v>
       </c>
       <c r="E160" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A161" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="B161" s="1" t="s">
         <v>69</v>
@@ -6306,12 +6310,12 @@
         <v>85</v>
       </c>
       <c r="E161" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A162" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="B162" s="1" t="s">
         <v>69</v>
@@ -6323,12 +6327,12 @@
         <v>80</v>
       </c>
       <c r="E162" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A163" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="B163" s="1" t="s">
         <v>69</v>
@@ -6340,12 +6344,12 @@
         <v>78</v>
       </c>
       <c r="E163" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A164" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="B164" s="1" t="s">
         <v>69</v>
@@ -6357,12 +6361,12 @@
         <v>71</v>
       </c>
       <c r="E164" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A165" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="B165" s="1" t="s">
         <v>69</v>
@@ -6374,12 +6378,12 @@
         <v>82</v>
       </c>
       <c r="E165" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A166" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="B166" s="1" t="s">
         <v>69</v>
@@ -6391,12 +6395,12 @@
         <v>86</v>
       </c>
       <c r="E166" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A167" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="B167" s="1" t="s">
         <v>69</v>
@@ -6408,12 +6412,12 @@
         <v>85</v>
       </c>
       <c r="E167" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A168" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="B168" s="1" t="s">
         <v>69</v>
@@ -6425,12 +6429,12 @@
         <v>80</v>
       </c>
       <c r="E168" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A169" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="B169" s="1" t="s">
         <v>69</v>
@@ -6442,12 +6446,12 @@
         <v>78</v>
       </c>
       <c r="E169" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A170" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="B170" s="1" t="s">
         <v>69</v>
@@ -6459,12 +6463,12 @@
         <v>71</v>
       </c>
       <c r="E170" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A171" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="B171" s="1" t="s">
         <v>69</v>
@@ -6476,12 +6480,12 @@
         <v>82</v>
       </c>
       <c r="E171" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A172" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="B172" s="1" t="s">
         <v>69</v>
@@ -6493,12 +6497,12 @@
         <v>86</v>
       </c>
       <c r="E172" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A173" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="B173" s="1" t="s">
         <v>69</v>
@@ -6510,12 +6514,12 @@
         <v>85</v>
       </c>
       <c r="E173" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A174" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="B174" s="1" t="s">
         <v>69</v>
@@ -6527,12 +6531,12 @@
         <v>80</v>
       </c>
       <c r="E174" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A175" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="B175" s="1" t="s">
         <v>69</v>
@@ -6544,12 +6548,12 @@
         <v>78</v>
       </c>
       <c r="E175" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A176" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B176" s="1" t="s">
         <v>69</v>
@@ -6561,12 +6565,12 @@
         <v>71</v>
       </c>
       <c r="E176" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A177" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B177" s="1" t="s">
         <v>69</v>
@@ -6578,12 +6582,12 @@
         <v>82</v>
       </c>
       <c r="E177" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A178" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B178" s="1" t="s">
         <v>69</v>
@@ -6595,12 +6599,12 @@
         <v>86</v>
       </c>
       <c r="E178" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A179" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B179" s="1" t="s">
         <v>69</v>
@@ -6612,12 +6616,12 @@
         <v>85</v>
       </c>
       <c r="E179" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A180" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B180" s="1" t="s">
         <v>69</v>
@@ -6629,12 +6633,12 @@
         <v>80</v>
       </c>
       <c r="E180" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A181" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B181" s="1" t="s">
         <v>69</v>
@@ -6646,12 +6650,12 @@
         <v>78</v>
       </c>
       <c r="E181" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A182" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="B182" s="1" t="s">
         <v>69</v>
@@ -6663,12 +6667,12 @@
         <v>71</v>
       </c>
       <c r="E182" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A183" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="B183" s="1" t="s">
         <v>69</v>
@@ -6680,12 +6684,12 @@
         <v>82</v>
       </c>
       <c r="E183" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A184" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="B184" s="1" t="s">
         <v>69</v>
@@ -6697,12 +6701,12 @@
         <v>86</v>
       </c>
       <c r="E184" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A185" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="B185" s="1" t="s">
         <v>69</v>
@@ -6714,12 +6718,12 @@
         <v>85</v>
       </c>
       <c r="E185" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A186" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="B186" s="1" t="s">
         <v>69</v>
@@ -6731,12 +6735,12 @@
         <v>80</v>
       </c>
       <c r="E186" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A187" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="B187" s="1" t="s">
         <v>69</v>
@@ -6748,12 +6752,12 @@
         <v>78</v>
       </c>
       <c r="E187" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A188" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="B188" s="1" t="s">
         <v>69</v>
@@ -6765,12 +6769,12 @@
         <v>71</v>
       </c>
       <c r="E188" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A189" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="B189" s="1" t="s">
         <v>69</v>
@@ -6782,12 +6786,12 @@
         <v>82</v>
       </c>
       <c r="E189" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A190" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="B190" s="1" t="s">
         <v>69</v>
@@ -6799,12 +6803,12 @@
         <v>86</v>
       </c>
       <c r="E190" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A191" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="B191" s="1" t="s">
         <v>69</v>
@@ -6816,12 +6820,12 @@
         <v>85</v>
       </c>
       <c r="E191" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A192" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="B192" s="1" t="s">
         <v>69</v>
@@ -6833,12 +6837,12 @@
         <v>80</v>
       </c>
       <c r="E192" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A193" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="B193" s="1" t="s">
         <v>69</v>
@@ -6850,12 +6854,12 @@
         <v>78</v>
       </c>
       <c r="E193" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A194" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="B194" s="1" t="s">
         <v>69</v>
@@ -6867,12 +6871,12 @@
         <v>71</v>
       </c>
       <c r="E194" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A195" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="B195" s="1" t="s">
         <v>69</v>
@@ -6884,12 +6888,12 @@
         <v>82</v>
       </c>
       <c r="E195" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A196" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="B196" s="1" t="s">
         <v>69</v>
@@ -6901,12 +6905,12 @@
         <v>86</v>
       </c>
       <c r="E196" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A197" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="B197" s="1" t="s">
         <v>69</v>
@@ -6918,12 +6922,12 @@
         <v>85</v>
       </c>
       <c r="E197" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A198" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="B198" s="1" t="s">
         <v>69</v>
@@ -6935,12 +6939,12 @@
         <v>80</v>
       </c>
       <c r="E198" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A199" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="B199" s="1" t="s">
         <v>69</v>
@@ -6952,12 +6956,12 @@
         <v>78</v>
       </c>
       <c r="E199" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A200" t="s">
-        <v>2</v>
+        <v>58</v>
       </c>
       <c r="B200" s="1" t="s">
         <v>69</v>
@@ -6969,12 +6973,12 @@
         <v>71</v>
       </c>
       <c r="E200" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A201" t="s">
-        <v>2</v>
+        <v>58</v>
       </c>
       <c r="B201" s="1" t="s">
         <v>69</v>
@@ -6986,12 +6990,12 @@
         <v>82</v>
       </c>
       <c r="E201" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A202" t="s">
-        <v>2</v>
+        <v>58</v>
       </c>
       <c r="B202" s="1" t="s">
         <v>69</v>
@@ -7003,12 +7007,12 @@
         <v>86</v>
       </c>
       <c r="E202" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A203" t="s">
-        <v>2</v>
+        <v>58</v>
       </c>
       <c r="B203" s="1" t="s">
         <v>69</v>
@@ -7020,12 +7024,12 @@
         <v>85</v>
       </c>
       <c r="E203" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A204" t="s">
-        <v>2</v>
+        <v>58</v>
       </c>
       <c r="B204" s="1" t="s">
         <v>69</v>
@@ -7037,12 +7041,12 @@
         <v>80</v>
       </c>
       <c r="E204" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A205" t="s">
-        <v>2</v>
+        <v>58</v>
       </c>
       <c r="B205" s="1" t="s">
         <v>69</v>
@@ -7054,12 +7058,12 @@
         <v>78</v>
       </c>
       <c r="E205" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A206" t="s">
-        <v>140</v>
+        <v>46</v>
       </c>
       <c r="B206" s="1" t="s">
         <v>69</v>
@@ -7067,16 +7071,16 @@
       <c r="C206" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D206" t="s">
-        <v>139</v>
+      <c r="D206" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="E206" t="s">
-        <v>149</v>
+        <v>47</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A207" t="s">
-        <v>140</v>
+        <v>46</v>
       </c>
       <c r="B207" s="1" t="s">
         <v>69</v>
@@ -7084,16 +7088,16 @@
       <c r="C207" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D207" t="s">
-        <v>81</v>
+      <c r="D207" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="E207" t="s">
-        <v>149</v>
+        <v>47</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A208" t="s">
-        <v>140</v>
+        <v>46</v>
       </c>
       <c r="B208" s="1" t="s">
         <v>69</v>
@@ -7101,16 +7105,16 @@
       <c r="C208" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D208" t="s">
-        <v>83</v>
+      <c r="D208" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="E208" t="s">
-        <v>149</v>
+        <v>47</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A209" t="s">
-        <v>140</v>
+        <v>46</v>
       </c>
       <c r="B209" s="1" t="s">
         <v>69</v>
@@ -7118,16 +7122,16 @@
       <c r="C209" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D209" t="s">
-        <v>84</v>
+      <c r="D209" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="E209" t="s">
-        <v>149</v>
+        <v>47</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A210" t="s">
-        <v>140</v>
+        <v>46</v>
       </c>
       <c r="B210" s="1" t="s">
         <v>69</v>
@@ -7135,16 +7139,16 @@
       <c r="C210" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D210" t="s">
-        <v>79</v>
+      <c r="D210" s="1" t="s">
+        <v>80</v>
       </c>
       <c r="E210" t="s">
-        <v>149</v>
+        <v>47</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A211" t="s">
-        <v>140</v>
+        <v>46</v>
       </c>
       <c r="B211" s="1" t="s">
         <v>69</v>
@@ -7152,16 +7156,16 @@
       <c r="C211" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D211" t="s">
-        <v>77</v>
+      <c r="D211" s="1" t="s">
+        <v>78</v>
       </c>
       <c r="E211" t="s">
-        <v>149</v>
+        <v>47</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A212" t="s">
-        <v>140</v>
+        <v>2</v>
       </c>
       <c r="B212" s="1" t="s">
         <v>69</v>
@@ -7169,16 +7173,16 @@
       <c r="C212" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D212" t="s">
-        <v>139</v>
+      <c r="D212" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="E212" t="s">
-        <v>150</v>
+        <v>3</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A213" t="s">
-        <v>140</v>
+        <v>2</v>
       </c>
       <c r="B213" s="1" t="s">
         <v>69</v>
@@ -7186,16 +7190,16 @@
       <c r="C213" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D213" t="s">
-        <v>81</v>
+      <c r="D213" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="E213" t="s">
-        <v>150</v>
+        <v>3</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A214" t="s">
-        <v>140</v>
+        <v>2</v>
       </c>
       <c r="B214" s="1" t="s">
         <v>69</v>
@@ -7203,16 +7207,16 @@
       <c r="C214" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D214" t="s">
-        <v>83</v>
+      <c r="D214" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="E214" t="s">
-        <v>150</v>
+        <v>3</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A215" t="s">
-        <v>140</v>
+        <v>2</v>
       </c>
       <c r="B215" s="1" t="s">
         <v>69</v>
@@ -7220,16 +7224,16 @@
       <c r="C215" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D215" t="s">
-        <v>84</v>
+      <c r="D215" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="E215" t="s">
-        <v>150</v>
+        <v>3</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A216" t="s">
-        <v>140</v>
+        <v>2</v>
       </c>
       <c r="B216" s="1" t="s">
         <v>69</v>
@@ -7237,16 +7241,16 @@
       <c r="C216" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D216" t="s">
-        <v>79</v>
+      <c r="D216" s="1" t="s">
+        <v>80</v>
       </c>
       <c r="E216" t="s">
-        <v>150</v>
+        <v>3</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A217" t="s">
-        <v>140</v>
+        <v>2</v>
       </c>
       <c r="B217" s="1" t="s">
         <v>69</v>
@@ -7254,11 +7258,11 @@
       <c r="C217" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D217" t="s">
-        <v>77</v>
+      <c r="D217" s="1" t="s">
+        <v>78</v>
       </c>
       <c r="E217" t="s">
-        <v>150</v>
+        <v>3</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.15">
@@ -7275,7 +7279,7 @@
         <v>139</v>
       </c>
       <c r="E218" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.15">
@@ -7292,7 +7296,7 @@
         <v>81</v>
       </c>
       <c r="E219" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.15">
@@ -7309,7 +7313,7 @@
         <v>83</v>
       </c>
       <c r="E220" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.15">
@@ -7326,7 +7330,7 @@
         <v>84</v>
       </c>
       <c r="E221" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.15">
@@ -7343,7 +7347,7 @@
         <v>79</v>
       </c>
       <c r="E222" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.15">
@@ -7360,7 +7364,7 @@
         <v>77</v>
       </c>
       <c r="E223" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.15">
@@ -8180,7 +8184,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E205"/>
+  <autoFilter ref="A1:E217"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>